<commit_message>
android ws port - 30002
</commit_message>
<xml_diff>
--- a/socket/sample.xlsx
+++ b/socket/sample.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="11865" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="11865" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="init_data" sheetId="1" r:id="rId1"/>
     <sheet name="web1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="web_url_info" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>_C_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,6 +190,57 @@
   </si>
   <si>
     <t>send data - top</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_C_NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_C_HTML</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_C_UDP_PORT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_C_MACADDR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_CUSTOM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUSTOM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://iotc365.com/test_locale/socket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:08:22:d0:15:fc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_DISC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WEBDISC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://static.iotc365.cn/socket</t>
+  </si>
+  <si>
+    <t>web_url_info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:08:22:d0:15:fc1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -550,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -781,12 +832,72 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>11001</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3">
+        <v>11002</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>